<commit_message>
ib 8 9 10 11
</commit_message>
<xml_diff>
--- a/labs.xlsx
+++ b/labs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Solly\Documents\GitHub\Sem8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13D9975-15F1-44C7-AB0D-36BDDC8E03D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BD46A2-65A1-42C1-B57E-A52E01B75128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,20 +504,20 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
@@ -657,8 +657,8 @@
       <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="1">
-        <v>0</v>
+      <c r="K5" s="3">
+        <v>1</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -677,8 +677,8 @@
       <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
+      <c r="C6" s="3">
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -689,8 +689,8 @@
       <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="1">
-        <v>0</v>
+      <c r="G6" s="3">
+        <v>1</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -722,7 +722,7 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N9">
         <f>65-SUM(B2:N6)</f>
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>